<commit_message>
EPBDS-2195 Rem('%') operator for BigDecimalValue, BigIntegerValue
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/operators/RemOperatorTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/operators/RemOperatorTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="24">
   <si>
     <t>C1</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Rules String testRemDoubleValue(DoubleValue v1, DoubleValue v2)</t>
+  </si>
+  <si>
+    <t>Rules String testRemBigIntegerValue(BigIntegerValue v1, BigIntegerValue v2)</t>
+  </si>
+  <si>
+    <t>Rules String testRemBigDecimalValue(BigDecimalValue v1, BigDecimalValue v2)</t>
   </si>
 </sst>
 </file>
@@ -480,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B6:F62"/>
+  <dimension ref="B6:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1011,8 +1017,110 @@
         <v>10</v>
       </c>
     </row>
+    <row r="66" spans="5:6" ht="17.25">
+      <c r="E66" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="5:6">
+      <c r="E67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="5:6">
+      <c r="E68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="5:6">
+      <c r="E69" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="5:6" ht="17.25">
+      <c r="E70" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="5:6" ht="17.25">
+      <c r="E71" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="5:6" ht="17.25">
+      <c r="E72" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="5:6" ht="17.25">
+      <c r="E76" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="5:6">
+      <c r="E77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="5:6">
+      <c r="E78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F78" s="1"/>
+    </row>
+    <row r="79" spans="5:6">
+      <c r="E79" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79" s="1"/>
+    </row>
+    <row r="80" spans="5:6" ht="17.25">
+      <c r="E80" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="5:6" ht="17.25">
+      <c r="E81" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="5:6" ht="17.25">
+      <c r="E82" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E76:F76"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B6:C6"/>

</xml_diff>